<commit_message>
fix: rubber duck and data
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/AnimalCharacter.xlsx
+++ b/data/Spreadsheet_Data/AnimalCharacter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7513E348-DE58-0948-B116-C8C42DF6B04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92147A74-F852-7441-83AC-9C25A5854407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37720" yWindow="500" windowWidth="37460" windowHeight="31500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8580" yWindow="5640" windowWidth="23840" windowHeight="21760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -199,6 +199,108 @@
   </si>
   <si>
     <t xml:space="preserve">#a4f0ff, #ff0000, #ffffff, #adff5c, #3e589c, #521c32, #fff700  </t>
+  </si>
+  <si>
+    <t>Rita's duck</t>
+  </si>
+  <si>
+    <t>Ivan's duck</t>
+  </si>
+  <si>
+    <t>DanielaS's duck</t>
+  </si>
+  <si>
+    <t>Balduin's duck</t>
+  </si>
+  <si>
+    <t>Christian's duck</t>
+  </si>
+  <si>
+    <t>JulienS's duck</t>
+  </si>
+  <si>
+    <t>Johannes's duck</t>
+  </si>
+  <si>
+    <t>Florian's duck</t>
+  </si>
+  <si>
+    <t>Nora's duck</t>
+  </si>
+  <si>
+    <t>Gregor's duck</t>
+  </si>
+  <si>
+    <t>A_010</t>
+  </si>
+  <si>
+    <t>A_011</t>
+  </si>
+  <si>
+    <t>A_012</t>
+  </si>
+  <si>
+    <t>A_013</t>
+  </si>
+  <si>
+    <t>A_014</t>
+  </si>
+  <si>
+    <t>A_015</t>
+  </si>
+  <si>
+    <t>A_016</t>
+  </si>
+  <si>
+    <t>A_017</t>
+  </si>
+  <si>
+    <t>A_018</t>
+  </si>
+  <si>
+    <t>A_019</t>
+  </si>
+  <si>
+    <t>#62B9FF</t>
+  </si>
+  <si>
+    <t>#885D00, #FFFFFF, #991700, #050505, #40403E, #6D0813</t>
+  </si>
+  <si>
+    <t>#FFFFFF, #7C1000, #7F7B89, #D58A91, #F1DC00</t>
+  </si>
+  <si>
+    <t>#A51B38, #000000, #FFFFFF</t>
+  </si>
+  <si>
+    <t>#000000, #FFFFFF, #DFAB00, #F55723, #0DA5DD, #950003, #B6B3B4</t>
+  </si>
+  <si>
+    <t>#EEC900, #FFFFFF, #000000, #38061C, #EB370F, #1F0D06, #ECCA00</t>
+  </si>
+  <si>
+    <t>#A7141E, #000000, #FFFFFF, #F36137, #5E6BC5, #007657</t>
+  </si>
+  <si>
+    <t>#007476,  #000000, #FFFFFF, #D03100, #A5A19D</t>
+  </si>
+  <si>
+    <t>H_002</t>
+  </si>
+  <si>
+    <t>H_012</t>
+  </si>
+  <si>
+    <t>H_021</t>
+  </si>
+  <si>
+    <t>H_009</t>
+  </si>
+  <si>
+    <t>H_008</t>
+  </si>
+  <si>
+    <t>H_019</t>
   </si>
 </sst>
 </file>
@@ -486,10 +588,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -498,7 +600,7 @@
     <col min="3" max="3" width="24.1640625" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
     <col min="5" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="49.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="21.83203125" customWidth="1"/>
     <col min="10" max="13" width="21.1640625" customWidth="1"/>
     <col min="14" max="14" width="21.1640625" style="8" customWidth="1"/>
@@ -819,67 +921,240 @@
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
fix: data model and animalcharacter xlsx
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/AnimalCharacter.xlsx
+++ b/data/Spreadsheet_Data/AnimalCharacter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10B2B98-EA2C-7242-8CF0-455904260977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A5A101-3A1B-7144-8633-2E2DC38F19AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="8280" windowWidth="29100" windowHeight="21760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="3220" windowWidth="35740" windowHeight="26460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
   <si>
     <t>ID</t>
   </si>
@@ -46,9 +46,6 @@
     <t>H_013</t>
   </si>
   <si>
-    <t>Dog</t>
-  </si>
-  <si>
     <t>A_002</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
   </si>
   <si>
     <t>H_007</t>
-  </si>
-  <si>
-    <t>Cat</t>
   </si>
   <si>
     <t>A_007</t>
@@ -161,9 +155,6 @@
     <t>This Italian Greyhound is a bundle of affection, always eager to cuddle and stay close. He loves nothing more than snuggling by your side. His soulful eyes and tender presence bring comfort and joy wherever he goes.</t>
   </si>
   <si>
-    <t>This older female Miniature Pinscher, with her striking three-colored coat, enjoys the comfort of being in the same room as you, often indulging in long, peaceful naps. Despite her age, she remains alert and curious, especially outdoors where she loves to watch her surroundings and keenly hunts for mice</t>
-  </si>
-  <si>
     <t>A_002, A_003, A_004</t>
   </si>
   <si>
@@ -301,6 +292,46 @@
   </si>
   <si>
     <t>H_019</t>
+  </si>
+  <si>
+    <t>Ramon, a medium-sized dog resembling a fox, hails from Romania and is a charming mix of dachshund and German shepherd. He loves to sleep and enjoys hiking adventures—just don't ask him to choose between a nap and a walk, it's his "ruffest" decision!</t>
+  </si>
+  <si>
+    <t>Cute little Yorkshire Terrier-Maltese Mix, prefers to be cuddled all day. Every person in her line of sight is responsible to pay their dues in daily pets. She prefers human companionships as other dogs are not able to pet her.
+Apart from this she enjoys naps, the outdoors (but only in small doses) and chasing snow balls.</t>
+  </si>
+  <si>
+    <t>This older female Miniature Pinscher, with her striking three-colored coat, enjoys the comfort of being in the same room as you, often indulging in long, peaceful naps. Despite her age, she remains alert and curious, especially outdoors where she loves to watch her surroundings and keenly hunts for mice.</t>
+  </si>
+  <si>
+    <t>#ffffff, #000000, #808080, #F5F5DC</t>
+  </si>
+  <si>
+    <t>W_009</t>
+  </si>
+  <si>
+    <t>Swedish Vallhund</t>
+  </si>
+  <si>
+    <t>Yorkshire Terrier-Maltese Mix</t>
+  </si>
+  <si>
+    <t>Miniature Pinscher</t>
+  </si>
+  <si>
+    <t>Italian Greyhound</t>
+  </si>
+  <si>
+    <t>31/4/2015</t>
+  </si>
+  <si>
+    <t>Mixed-breed</t>
+  </si>
+  <si>
+    <t>European Shorthair</t>
+  </si>
+  <si>
+    <t>Mixed-breed dog</t>
   </si>
 </sst>
 </file>
@@ -590,8 +621,8 @@
   </sheetPr>
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -611,10 +642,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -623,16 +654,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -641,16 +672,16 @@
         <v>3</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -658,7 +689,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -668,93 +699,109 @@
       </c>
       <c r="F2" s="1"/>
       <c r="I2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
+        <v>48</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="1"/>
-      <c r="K3" s="1" t="s">
-        <v>8</v>
+      <c r="K3" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="I4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>8</v>
+        <v>48</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="N4" s="7"/>
+      <c r="N4" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F5" s="1"/>
       <c r="J5">
-        <v>5.5</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>8</v>
+        <v>4.7</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M5" s="1">
         <v>1</v>
@@ -765,29 +812,29 @@
     </row>
     <row r="6" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1"/>
       <c r="J6">
         <v>9</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>8</v>
+      <c r="K6" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M6" s="1">
         <v>1</v>
@@ -798,94 +845,94 @@
     </row>
     <row r="7" spans="1:15" ht="70" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J7">
         <v>3.6</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>23</v>
+      <c r="K7" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M7" s="1">
         <v>1</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" ht="56" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J8">
         <v>4.2</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>23</v>
+      <c r="K8" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M8" s="1">
         <v>1</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F9" s="1"/>
-      <c r="K9" s="1" t="s">
-        <v>23</v>
+      <c r="K9" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -893,240 +940,240 @@
     </row>
     <row r="10" spans="1:15" ht="64" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J10">
         <v>0.05</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="L11" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
fix: data model and list
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/AnimalCharacter.xlsx
+++ b/data/Spreadsheet_Data/AnimalCharacter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A5A101-3A1B-7144-8633-2E2DC38F19AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7D04B6-DE73-864A-8124-242053DEAE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="3220" windowWidth="35740" windowHeight="26460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3880" yWindow="5480" windowWidth="39860" windowHeight="26460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>Mixed-breed dog</t>
+  </si>
+  <si>
+    <t>This male Bengal cat is called Anubis. He is very curious, but shy.</t>
+  </si>
+  <si>
+    <t>Bengal Cat</t>
   </si>
 </sst>
 </file>
@@ -621,8 +627,8 @@
   </sheetPr>
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -927,14 +933,19 @@
       <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D9" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="1"/>
       <c r="K9" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L9" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="O9" s="1"/>
     </row>
@@ -980,6 +991,9 @@
       <c r="G11" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="J11">
+        <v>0.05</v>
+      </c>
       <c r="K11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1000,6 +1014,9 @@
       <c r="G12" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="J12">
+        <v>0.05</v>
+      </c>
       <c r="K12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1020,6 +1037,9 @@
       <c r="G13" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="J13">
+        <v>0.05</v>
+      </c>
       <c r="K13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1040,6 +1060,9 @@
       <c r="G14" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="J14">
+        <v>0.05</v>
+      </c>
       <c r="K14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1060,6 +1083,9 @@
       <c r="G15" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="J15">
+        <v>0.05</v>
+      </c>
       <c r="K15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1080,6 +1106,9 @@
       <c r="G16" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="J16">
+        <v>0.05</v>
+      </c>
       <c r="K16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1100,6 +1129,9 @@
       <c r="G17" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="J17">
+        <v>0.05</v>
+      </c>
       <c r="K17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1120,6 +1152,9 @@
       <c r="G18" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="J18">
+        <v>0.05</v>
+      </c>
       <c r="K18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1140,6 +1175,9 @@
       <c r="G19" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="J19">
+        <v>0.05</v>
+      </c>
       <c r="K19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1160,6 +1198,9 @@
       <c r="G20" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="J20">
+        <v>0.05</v>
+      </c>
       <c r="K20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1169,6 +1210,9 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
+      <c r="J21">
+        <v>0.05</v>
+      </c>
       <c r="K21" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
fix: add animal images
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/AnimalCharacter.xlsx
+++ b/data/Spreadsheet_Data/AnimalCharacter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A773E9E5-5DBC-784F-AFF7-D0B0B30ED2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ABB20C-485F-384A-A05E-AA0D4744A36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="2900" windowWidth="39860" windowHeight="26460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,9 +149,6 @@
     <t>Link to Flyer ID</t>
   </si>
   <si>
-    <t>A_004, A_004</t>
-  </si>
-  <si>
     <t>This Italian Greyhound is a bundle of affection, always eager to cuddle and stay close. He loves nothing more than snuggling by your side. His soulful eyes and tender presence bring comfort and joy wherever he goes.</t>
   </si>
   <si>
@@ -395,6 +392,9 @@
   </si>
   <si>
     <t>FL_004</t>
+  </si>
+  <si>
+    <t>A_004, A_001</t>
   </si>
 </sst>
 </file>
@@ -684,8 +684,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -705,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>32</v>
@@ -752,7 +751,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -762,18 +761,18 @@
       </c>
       <c r="F2" s="1"/>
       <c r="I2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="6"/>
       <c r="O2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -787,22 +786,22 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="1"/>
       <c r="K3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="6"/>
       <c r="O3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -816,37 +815,37 @@
         <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J4" s="2">
         <v>3.3</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -860,7 +859,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -870,10 +869,10 @@
         <v>4.7</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M5" s="1">
         <v>1</v>
@@ -882,7 +881,7 @@
         <v>40977</v>
       </c>
       <c r="O5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.15">
@@ -890,13 +889,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -906,10 +905,10 @@
         <v>9</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M6" s="1">
         <v>1</v>
@@ -918,7 +917,7 @@
         <v>44392</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="70" x14ac:dyDescent="0.15">
@@ -939,28 +938,28 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J7">
         <v>3.6</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M7" s="1">
         <v>1</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="56" x14ac:dyDescent="0.15">
@@ -981,25 +980,25 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J8">
         <v>4.2</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M8" s="1">
         <v>1</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1010,21 +1009,21 @@
         <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="1"/>
       <c r="K9" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="64" customHeight="1" x14ac:dyDescent="0.15">
@@ -1035,14 +1034,14 @@
         <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J10">
         <v>0.05</v>
@@ -1051,26 +1050,26 @@
         <v>28</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="6"/>
       <c r="O10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11">
         <v>0.05</v>
@@ -1079,24 +1078,24 @@
         <v>28</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J12">
         <v>0.05</v>
@@ -1105,24 +1104,24 @@
         <v>28</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J13">
         <v>0.05</v>
@@ -1131,24 +1130,24 @@
         <v>28</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J14">
         <v>0.05</v>
@@ -1157,24 +1156,24 @@
         <v>28</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J15">
         <v>0.05</v>
@@ -1183,24 +1182,24 @@
         <v>28</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J16">
         <v>0.05</v>
@@ -1209,24 +1208,24 @@
         <v>28</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J17">
         <v>0.05</v>
@@ -1235,24 +1234,24 @@
         <v>28</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J18">
         <v>0.05</v>
@@ -1261,24 +1260,24 @@
         <v>28</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J19">
         <v>0.05</v>
@@ -1287,24 +1286,24 @@
         <v>28</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20">
         <v>0.05</v>
@@ -1313,10 +1312,10 @@
         <v>28</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1328,7 +1327,7 @@
         <v>28</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>